<commit_message>
Updating insights and EDA files
</commit_message>
<xml_diff>
--- a/analysis_files/insights.xlsx
+++ b/analysis_files/insights.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhom Joshua\Documents\files\Data Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rhom Joshua\Documents\files\Data Analysis\portfolio_projects\Walmart-Sales-Data-Analysis\analysis_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B12408-C85B-473E-B08C-1E9E2DA54FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F016D783-C22C-446F-9F9D-FE70239CB290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="2" xr2:uid="{B11FB0F8-1C52-49AA-ADB7-88431B61E74C}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" firstSheet="1" activeTab="3" xr2:uid="{B11FB0F8-1C52-49AA-ADB7-88431B61E74C}"/>
   </bookViews>
   <sheets>
     <sheet name="trends_analysis" sheetId="2" r:id="rId1"/>
     <sheet name="city_revenue" sheetId="4" r:id="rId2"/>
     <sheet name="profitability" sheetId="5" r:id="rId3"/>
+    <sheet name="ratings" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>tab</t>
   </si>
@@ -234,6 +235,48 @@
   </si>
   <si>
     <t>Quantity - Profit Margin: r-squared = 0.000005, sales volume (quantity) and price don’t influence the margin.</t>
+  </si>
+  <si>
+    <t>Goal : Reveal customer preferences and operational/business opportunities.</t>
+  </si>
+  <si>
+    <t>Credit card transactions are the largest share, followed by E-wallets, then cash. This suggests that customers prefer digital transactions (credit card + E-wallet &gt; 70%).</t>
+  </si>
+  <si>
+    <t>Cash payments generate the lowest revenue and transaction volume, indicating it’s a less preferred method overall.</t>
+  </si>
+  <si>
+    <t>Most ratings cluster between 6 and 9, suggesting customers are generally satisfied, but very few rate extremely low or extremely high. The distribution is slightly skewed towards the higher side (positive experience overall).</t>
+  </si>
+  <si>
+    <t>Ratings peaked in early 2019, then steadily declined around 2020 and stabilized between 5.5 and 6.5. This indicates a gradual decrease in customer satisfaction over time.</t>
+  </si>
+  <si>
+    <t>Ewallet not only accounts for a large volume of transactions (8,932) but also has the highest customer satisfaction (avg. rating 6.48). Credit card has the largest quantity of sales (9,573), but its rating is significantly lower (5.42). Cash has both the lowest transaction count (5,077) and lowest rating (5.40).</t>
+  </si>
+  <si>
+    <t>Revenue is not strongly correlated with customer satisfaction. Example: Weslaco has the highest revenue (~$46K) but relatively low ratings (5.18). Meanwhile, Austin shows the highest rating (7.0) but generates only ~$7.5K in revenue.</t>
+  </si>
+  <si>
+    <t>walmart_cleaned.ratings</t>
+  </si>
+  <si>
+    <t>payment_method/quantity</t>
+  </si>
+  <si>
+    <t>rating/quantity</t>
+  </si>
+  <si>
+    <t>rating/datetime</t>
+  </si>
+  <si>
+    <t>rating/payment_method/quantity</t>
+  </si>
+  <si>
+    <t>total_revenue/city/rating</t>
+  </si>
+  <si>
+    <t>Sales/Marketing</t>
   </si>
 </sst>
 </file>
@@ -942,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B9FA40-9370-4CE6-8EA5-0F4949D785C1}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,4 +1114,143 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{327E77C0-61E8-490B-8C30-DFE5E1AE9706}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="4" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="2"/>
+    <col min="9" max="9" width="38.85546875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>